<commit_message>
MTP029 before cop row generation
</commit_message>
<xml_diff>
--- a/observations/orbit_plans/mtp029/nomad_mtp029_plan.xlsx
+++ b/observations/orbit_plans/mtp029/nomad_mtp029_plan.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\orbit_plans\mtp029\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F469BA-D066-4AB1-AEC0-FB9FA9D08A47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1839" uniqueCount="579">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1838" uniqueCount="579">
   <si>
     <t>#orbitType</t>
   </si>
@@ -1756,8 +1762,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1794,6 +1800,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1840,7 +1854,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1872,9 +1886,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1906,6 +1938,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2081,14 +2131,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M342"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A134" workbookViewId="0">
+      <selection activeCell="G140" sqref="G140"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2129,7 +2181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>3</v>
       </c>
@@ -2146,7 +2198,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2178,7 +2230,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>14</v>
       </c>
@@ -2192,7 +2244,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2227,7 +2279,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>14</v>
       </c>
@@ -2241,7 +2293,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2273,7 +2325,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2308,7 +2360,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:13">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>17</v>
       </c>
@@ -2325,7 +2377,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:13">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2357,7 +2409,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:13">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>14</v>
       </c>
@@ -2371,7 +2423,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>14</v>
       </c>
@@ -2385,7 +2437,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="13" spans="1:13">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2420,7 +2472,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:13">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>14</v>
       </c>
@@ -2434,7 +2486,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:13">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2469,7 +2521,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:13">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2501,7 +2553,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:13">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>14</v>
       </c>
@@ -2515,7 +2567,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:13">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
@@ -2550,7 +2602,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:13">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>14</v>
       </c>
@@ -2564,7 +2616,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:13">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2596,7 +2648,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:13">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2613,7 +2665,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:13">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2648,7 +2700,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:13">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2680,7 +2732,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="24" spans="1:13">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>14</v>
       </c>
@@ -2694,7 +2746,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="25" spans="1:13">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2711,7 +2763,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:13">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>1</v>
       </c>
@@ -2743,7 +2795,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="27" spans="1:13">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>14</v>
       </c>
@@ -2757,7 +2809,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="28" spans="1:13">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
@@ -2792,7 +2844,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:13">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2824,7 +2876,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="30" spans="1:13">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>14</v>
       </c>
@@ -2838,7 +2890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:13">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>1</v>
       </c>
@@ -2873,7 +2925,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="32" spans="1:13">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>14</v>
       </c>
@@ -2887,7 +2939,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2922,7 +2974,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
@@ -2954,7 +3006,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>17</v>
       </c>
@@ -2971,7 +3023,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>1</v>
       </c>
@@ -3006,7 +3058,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>14</v>
       </c>
@@ -3020,7 +3072,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>14</v>
       </c>
@@ -3034,7 +3086,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>1</v>
       </c>
@@ -3069,7 +3121,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>14</v>
       </c>
@@ -3083,7 +3135,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>1</v>
       </c>
@@ -3115,7 +3167,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="42" spans="1:13">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>1</v>
       </c>
@@ -3147,7 +3199,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="43" spans="1:13">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>3</v>
       </c>
@@ -3164,7 +3216,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:13">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>1</v>
       </c>
@@ -3196,7 +3248,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:13">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>14</v>
       </c>
@@ -3210,7 +3262,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="46" spans="1:13">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>1</v>
       </c>
@@ -3245,7 +3297,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:13">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>17</v>
       </c>
@@ -3262,7 +3314,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="48" spans="1:13">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>1</v>
       </c>
@@ -3294,7 +3346,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3326,7 +3378,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>3</v>
       </c>
@@ -3343,7 +3395,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>14</v>
       </c>
@@ -3357,7 +3409,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="52" spans="1:13">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>1</v>
       </c>
@@ -3389,7 +3441,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="53" spans="1:13">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>14</v>
       </c>
@@ -3403,7 +3455,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:13">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>1</v>
       </c>
@@ -3438,7 +3490,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="55" spans="1:13">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>1</v>
       </c>
@@ -3470,7 +3522,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="56" spans="1:13">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>3</v>
       </c>
@@ -3487,7 +3539,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="57" spans="1:13">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>1</v>
       </c>
@@ -3519,7 +3571,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="58" spans="1:13">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>17</v>
       </c>
@@ -3539,7 +3591,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:13">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>1</v>
       </c>
@@ -3571,7 +3623,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="60" spans="1:13">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>1</v>
       </c>
@@ -3603,7 +3655,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="1:13">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>14</v>
       </c>
@@ -3617,7 +3669,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="62" spans="1:13">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>14</v>
       </c>
@@ -3631,7 +3683,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="63" spans="1:13">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>1</v>
       </c>
@@ -3666,7 +3718,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="64" spans="1:13">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>14</v>
       </c>
@@ -3680,7 +3732,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="65" spans="1:13">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>1</v>
       </c>
@@ -3712,7 +3764,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="66" spans="1:13">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>14</v>
       </c>
@@ -3726,7 +3778,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="67" spans="1:13">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>3</v>
       </c>
@@ -3743,7 +3795,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="68" spans="1:13">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>14</v>
       </c>
@@ -3757,7 +3809,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="69" spans="1:13">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>1</v>
       </c>
@@ -3789,7 +3841,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="70" spans="1:13">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>1</v>
       </c>
@@ -3824,7 +3876,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="71" spans="1:13">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>17</v>
       </c>
@@ -3841,7 +3893,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="72" spans="1:13">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>1</v>
       </c>
@@ -3873,7 +3925,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="73" spans="1:13">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>14</v>
       </c>
@@ -3887,7 +3939,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="74" spans="1:13">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>3</v>
       </c>
@@ -3904,7 +3956,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="75" spans="1:13">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>1</v>
       </c>
@@ -3936,7 +3988,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="76" spans="1:13">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>3</v>
       </c>
@@ -3953,7 +4005,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="77" spans="1:13">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>1</v>
       </c>
@@ -3976,7 +4028,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="78" spans="1:13">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>1</v>
       </c>
@@ -3999,7 +4051,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="79" spans="1:13">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>14</v>
       </c>
@@ -4013,7 +4065,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="80" spans="1:13">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>1</v>
       </c>
@@ -4039,7 +4091,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:13">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>14</v>
       </c>
@@ -4053,7 +4105,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="82" spans="1:13">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>1</v>
       </c>
@@ -4079,7 +4131,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="83" spans="1:13">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>1</v>
       </c>
@@ -4102,7 +4154,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="84" spans="1:13">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>17</v>
       </c>
@@ -4119,7 +4171,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="85" spans="1:13">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>28</v>
       </c>
@@ -4136,7 +4188,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="86" spans="1:13">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>14</v>
       </c>
@@ -4147,7 +4199,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="87" spans="1:13">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>14</v>
       </c>
@@ -4158,7 +4210,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="88" spans="1:13">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>3</v>
       </c>
@@ -4175,7 +4227,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="89" spans="1:13">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>1</v>
       </c>
@@ -4198,7 +4250,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="90" spans="1:13">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>14</v>
       </c>
@@ -4212,7 +4264,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="91" spans="1:13">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>1</v>
       </c>
@@ -4235,7 +4287,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="92" spans="1:13">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>1</v>
       </c>
@@ -4261,7 +4313,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:13">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>14</v>
       </c>
@@ -4275,7 +4327,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:13">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>1</v>
       </c>
@@ -4298,7 +4350,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:13">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>14</v>
       </c>
@@ -4312,7 +4364,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="96" spans="1:13">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>1</v>
       </c>
@@ -4338,7 +4390,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="97" spans="1:13">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>17</v>
       </c>
@@ -4355,7 +4407,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="98" spans="1:13">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>1</v>
       </c>
@@ -4381,7 +4433,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="1:13">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>14</v>
       </c>
@@ -4395,7 +4447,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="100" spans="1:13">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>1</v>
       </c>
@@ -4418,7 +4470,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="101" spans="1:13">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>8</v>
       </c>
@@ -4435,7 +4487,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="102" spans="1:13">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>1</v>
       </c>
@@ -4458,7 +4510,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="103" spans="1:13">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>14</v>
       </c>
@@ -4472,7 +4524,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="104" spans="1:13">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>1</v>
       </c>
@@ -4495,7 +4547,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="105" spans="1:13">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>3</v>
       </c>
@@ -4512,7 +4564,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="106" spans="1:13">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>1</v>
       </c>
@@ -4535,7 +4587,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="107" spans="1:13">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>1</v>
       </c>
@@ -4561,7 +4613,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="108" spans="1:13">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>14</v>
       </c>
@@ -4575,7 +4627,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="109" spans="1:13">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>1</v>
       </c>
@@ -4598,7 +4650,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="110" spans="1:13">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>17</v>
       </c>
@@ -4615,7 +4667,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="111" spans="1:13">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>1</v>
       </c>
@@ -4641,7 +4693,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="112" spans="1:13">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>14</v>
       </c>
@@ -4655,7 +4707,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="113" spans="1:13">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>1</v>
       </c>
@@ -4681,7 +4733,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="114" spans="1:13">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>14</v>
       </c>
@@ -4695,7 +4747,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="115" spans="1:13">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>1</v>
       </c>
@@ -4718,7 +4770,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="116" spans="1:13">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>14</v>
       </c>
@@ -4732,7 +4784,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="117" spans="1:13">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>1</v>
       </c>
@@ -4758,7 +4810,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="118" spans="1:13">
+    <row r="118" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>1</v>
       </c>
@@ -4781,7 +4833,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="119" spans="1:13">
+    <row r="119" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>14</v>
       </c>
@@ -4795,7 +4847,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="120" spans="1:13">
+    <row r="120" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>1</v>
       </c>
@@ -4821,7 +4873,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="121" spans="1:13">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>17</v>
       </c>
@@ -4838,7 +4890,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="122" spans="1:13">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>1</v>
       </c>
@@ -4861,7 +4913,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="123" spans="1:13">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>14</v>
       </c>
@@ -4875,7 +4927,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="124" spans="1:13">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>1</v>
       </c>
@@ -4901,7 +4953,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="125" spans="1:13">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>1</v>
       </c>
@@ -4924,7 +4976,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="126" spans="1:13">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>14</v>
       </c>
@@ -4938,7 +4990,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="127" spans="1:13">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>1</v>
       </c>
@@ -4964,7 +5016,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="128" spans="1:13">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>14</v>
       </c>
@@ -4978,7 +5030,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="129" spans="1:13">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>1</v>
       </c>
@@ -5001,7 +5053,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="130" spans="1:13">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>3</v>
       </c>
@@ -5018,7 +5070,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="131" spans="1:13">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>1</v>
       </c>
@@ -5041,7 +5093,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="132" spans="1:13">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>1</v>
       </c>
@@ -5067,7 +5119,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="133" spans="1:13">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>14</v>
       </c>
@@ -5081,13 +5133,10 @@
         <v>262</v>
       </c>
     </row>
-    <row r="134" spans="1:13">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>17</v>
       </c>
-      <c r="H134" t="s">
-        <v>67</v>
-      </c>
       <c r="I134" t="s">
         <v>8</v>
       </c>
@@ -5101,7 +5150,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="135" spans="1:13">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>14</v>
       </c>
@@ -5115,7 +5164,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="136" spans="1:13">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>1</v>
       </c>
@@ -5138,7 +5187,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="137" spans="1:13">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>3</v>
       </c>
@@ -5155,7 +5204,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="138" spans="1:13">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>14</v>
       </c>
@@ -5169,7 +5218,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="139" spans="1:13">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>1</v>
       </c>
@@ -5192,7 +5241,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="140" spans="1:13">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>1</v>
       </c>
@@ -5218,7 +5267,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="141" spans="1:13">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>14</v>
       </c>
@@ -5232,7 +5281,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="142" spans="1:13">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>1</v>
       </c>
@@ -5258,7 +5307,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="143" spans="1:13">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>14</v>
       </c>
@@ -5272,7 +5321,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="144" spans="1:13">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>1</v>
       </c>
@@ -5298,7 +5347,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="145" spans="1:13">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>1</v>
       </c>
@@ -5321,7 +5370,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="146" spans="1:13">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>17</v>
       </c>
@@ -5338,7 +5387,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="147" spans="1:13">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>1</v>
       </c>
@@ -5364,7 +5413,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="148" spans="1:13">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>14</v>
       </c>
@@ -5378,7 +5427,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="149" spans="1:13">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>1</v>
       </c>
@@ -5404,7 +5453,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="150" spans="1:13">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>14</v>
       </c>
@@ -5418,7 +5467,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="151" spans="1:13">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>1</v>
       </c>
@@ -5441,7 +5490,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="152" spans="1:13">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>1</v>
       </c>
@@ -5467,7 +5516,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="153" spans="1:13">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>14</v>
       </c>
@@ -5481,7 +5530,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="154" spans="1:13">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>1</v>
       </c>
@@ -5504,7 +5553,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="155" spans="1:13">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>14</v>
       </c>
@@ -5518,7 +5567,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="156" spans="1:13">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>1</v>
       </c>
@@ -5544,7 +5593,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="157" spans="1:13">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>14</v>
       </c>
@@ -5558,7 +5607,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="158" spans="1:13">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>1</v>
       </c>
@@ -5581,7 +5630,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="159" spans="1:13">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>1</v>
       </c>
@@ -5607,7 +5656,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="160" spans="1:13">
+    <row r="160" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>17</v>
       </c>
@@ -5624,7 +5673,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="161" spans="1:13">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>1</v>
       </c>
@@ -5650,7 +5699,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="162" spans="1:13">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>14</v>
       </c>
@@ -5664,7 +5713,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="163" spans="1:13">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>14</v>
       </c>
@@ -5678,7 +5727,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="164" spans="1:13">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>1</v>
       </c>
@@ -5704,7 +5753,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="165" spans="1:13">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>1</v>
       </c>
@@ -5727,7 +5776,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="166" spans="1:13">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>3</v>
       </c>
@@ -5744,7 +5793,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="167" spans="1:13">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>1</v>
       </c>
@@ -5767,7 +5816,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="168" spans="1:13">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>14</v>
       </c>
@@ -5781,7 +5830,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="169" spans="1:13">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>1</v>
       </c>
@@ -5807,7 +5856,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="170" spans="1:13">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>1</v>
       </c>
@@ -5830,7 +5879,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="171" spans="1:13">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>47</v>
       </c>
@@ -5850,7 +5899,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="172" spans="1:13">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>14</v>
       </c>
@@ -5861,7 +5910,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="173" spans="1:13">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>3</v>
       </c>
@@ -5878,7 +5927,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="174" spans="1:13">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>14</v>
       </c>
@@ -5892,7 +5941,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="175" spans="1:13">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>3</v>
       </c>
@@ -5909,7 +5958,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="176" spans="1:13">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>1</v>
       </c>
@@ -5932,7 +5981,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="177" spans="1:13">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>14</v>
       </c>
@@ -5946,7 +5995,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="178" spans="1:13">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>1</v>
       </c>
@@ -5972,7 +6021,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="179" spans="1:13">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>14</v>
       </c>
@@ -5986,7 +6035,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="180" spans="1:13">
+    <row r="180" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>1</v>
       </c>
@@ -6009,7 +6058,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="181" spans="1:13">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>1</v>
       </c>
@@ -6035,7 +6084,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="182" spans="1:13">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>14</v>
       </c>
@@ -6049,7 +6098,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="183" spans="1:13">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>1</v>
       </c>
@@ -6072,7 +6121,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="184" spans="1:13">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>7</v>
       </c>
@@ -6092,7 +6141,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="185" spans="1:13">
+    <row r="185" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>3</v>
       </c>
@@ -6109,7 +6158,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="186" spans="1:13">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>14</v>
       </c>
@@ -6123,7 +6172,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="187" spans="1:13">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>1</v>
       </c>
@@ -6146,7 +6195,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="188" spans="1:13">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>14</v>
       </c>
@@ -6160,7 +6209,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="189" spans="1:13">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>1</v>
       </c>
@@ -6186,7 +6235,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="190" spans="1:13">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>1</v>
       </c>
@@ -6209,7 +6258,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="191" spans="1:13">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>14</v>
       </c>
@@ -6223,7 +6272,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="192" spans="1:13">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>1</v>
       </c>
@@ -6249,7 +6298,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="193" spans="1:13">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>14</v>
       </c>
@@ -6263,7 +6312,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="194" spans="1:13">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>1</v>
       </c>
@@ -6286,7 +6335,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="195" spans="1:13">
+    <row r="195" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>1</v>
       </c>
@@ -6312,7 +6361,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="196" spans="1:13">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>17</v>
       </c>
@@ -6329,7 +6378,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="197" spans="1:13">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>1</v>
       </c>
@@ -6352,7 +6401,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="198" spans="1:13">
+    <row r="198" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>14</v>
       </c>
@@ -6366,7 +6415,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="199" spans="1:13">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>3</v>
       </c>
@@ -6383,7 +6432,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="200" spans="1:13">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>1</v>
       </c>
@@ -6406,7 +6455,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="201" spans="1:13">
+    <row r="201" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>1</v>
       </c>
@@ -6432,7 +6481,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="202" spans="1:13">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A202">
         <v>14</v>
       </c>
@@ -6446,7 +6495,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="203" spans="1:13">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A203">
         <v>1</v>
       </c>
@@ -6469,7 +6518,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="204" spans="1:13">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A204">
         <v>3</v>
       </c>
@@ -6486,7 +6535,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="205" spans="1:13">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A205">
         <v>1</v>
       </c>
@@ -6509,7 +6558,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="206" spans="1:13">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A206">
         <v>14</v>
       </c>
@@ -6523,7 +6572,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="207" spans="1:13">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A207">
         <v>1</v>
       </c>
@@ -6549,7 +6598,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="208" spans="1:13">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A208">
         <v>1</v>
       </c>
@@ -6572,7 +6621,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="209" spans="1:13">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A209">
         <v>17</v>
       </c>
@@ -6589,7 +6638,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="210" spans="1:13">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A210">
         <v>1</v>
       </c>
@@ -6612,7 +6661,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="211" spans="1:13">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A211">
         <v>3</v>
       </c>
@@ -6629,7 +6678,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="212" spans="1:13">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A212">
         <v>1</v>
       </c>
@@ -6652,7 +6701,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="213" spans="1:13">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A213">
         <v>8</v>
       </c>
@@ -6669,7 +6718,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="214" spans="1:13">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A214">
         <v>1</v>
       </c>
@@ -6692,7 +6741,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="215" spans="1:13">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A215">
         <v>1</v>
       </c>
@@ -6715,7 +6764,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="216" spans="1:13">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A216">
         <v>3</v>
       </c>
@@ -6732,7 +6781,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="217" spans="1:13">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A217">
         <v>1</v>
       </c>
@@ -6755,7 +6804,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="218" spans="1:13">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A218">
         <v>14</v>
       </c>
@@ -6769,7 +6818,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="219" spans="1:13">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A219">
         <v>1</v>
       </c>
@@ -6795,7 +6844,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="220" spans="1:13">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>1</v>
       </c>
@@ -6818,7 +6867,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="221" spans="1:13">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>47</v>
       </c>
@@ -6838,7 +6887,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="222" spans="1:13">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>14</v>
       </c>
@@ -6852,7 +6901,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="223" spans="1:13">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>3</v>
       </c>
@@ -6869,7 +6918,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="224" spans="1:13">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>14</v>
       </c>
@@ -6883,7 +6932,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="225" spans="1:13">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>1</v>
       </c>
@@ -6906,7 +6955,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="226" spans="1:13">
+    <row r="226" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>14</v>
       </c>
@@ -6920,7 +6969,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="227" spans="1:13">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>1</v>
       </c>
@@ -6946,7 +6995,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="228" spans="1:13">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>1</v>
       </c>
@@ -6969,7 +7018,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="229" spans="1:13">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>14</v>
       </c>
@@ -6983,7 +7032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="230" spans="1:13">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>1</v>
       </c>
@@ -7009,7 +7058,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="231" spans="1:13">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>14</v>
       </c>
@@ -7023,7 +7072,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="232" spans="1:13">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>1</v>
       </c>
@@ -7049,7 +7098,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="233" spans="1:13">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>17</v>
       </c>
@@ -7066,7 +7115,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="234" spans="1:13">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>1</v>
       </c>
@@ -7089,7 +7138,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="235" spans="1:13">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>1</v>
       </c>
@@ -7115,7 +7164,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="236" spans="1:13">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>14</v>
       </c>
@@ -7129,7 +7178,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="237" spans="1:13">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>1</v>
       </c>
@@ -7152,7 +7201,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="238" spans="1:13">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>14</v>
       </c>
@@ -7166,7 +7215,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="239" spans="1:13">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>1</v>
       </c>
@@ -7192,7 +7241,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="240" spans="1:13">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>14</v>
       </c>
@@ -7206,7 +7255,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="241" spans="1:13">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>1</v>
       </c>
@@ -7229,7 +7278,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="242" spans="1:13">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>1</v>
       </c>
@@ -7255,7 +7304,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="243" spans="1:13">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>14</v>
       </c>
@@ -7269,7 +7318,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="244" spans="1:13">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>1</v>
       </c>
@@ -7295,7 +7344,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="245" spans="1:13">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>17</v>
       </c>
@@ -7312,7 +7361,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="246" spans="1:13">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>1</v>
       </c>
@@ -7338,7 +7387,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="247" spans="1:13">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>1</v>
       </c>
@@ -7361,7 +7410,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="248" spans="1:13">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>14</v>
       </c>
@@ -7375,7 +7424,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="249" spans="1:13">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>3</v>
       </c>
@@ -7392,7 +7441,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="250" spans="1:13">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>1</v>
       </c>
@@ -7415,7 +7464,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="251" spans="1:13">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>14</v>
       </c>
@@ -7429,7 +7478,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="252" spans="1:13">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>1</v>
       </c>
@@ -7455,7 +7504,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="253" spans="1:13">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>1</v>
       </c>
@@ -7478,7 +7527,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="254" spans="1:13">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>14</v>
       </c>
@@ -7492,7 +7541,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="255" spans="1:13">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>1</v>
       </c>
@@ -7518,7 +7567,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="256" spans="1:13">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>14</v>
       </c>
@@ -7532,7 +7581,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="257" spans="1:13">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>14</v>
       </c>
@@ -7543,7 +7592,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="258" spans="1:13">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>14</v>
       </c>
@@ -7554,7 +7603,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="259" spans="1:13">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>17</v>
       </c>
@@ -7574,7 +7623,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="260" spans="1:13">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>1</v>
       </c>
@@ -7597,7 +7646,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="261" spans="1:13">
+    <row r="261" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>14</v>
       </c>
@@ -7611,7 +7660,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="262" spans="1:13">
+    <row r="262" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>3</v>
       </c>
@@ -7628,7 +7677,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="263" spans="1:13">
+    <row r="263" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>1</v>
       </c>
@@ -7651,7 +7700,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="264" spans="1:13">
+    <row r="264" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>1</v>
       </c>
@@ -7677,7 +7726,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="265" spans="1:13">
+    <row r="265" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>14</v>
       </c>
@@ -7691,7 +7740,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="266" spans="1:13">
+    <row r="266" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>1</v>
       </c>
@@ -7714,7 +7763,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="267" spans="1:13">
+    <row r="267" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>8</v>
       </c>
@@ -7731,7 +7780,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="268" spans="1:13">
+    <row r="268" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>1</v>
       </c>
@@ -7754,7 +7803,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="269" spans="1:13">
+    <row r="269" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>14</v>
       </c>
@@ -7768,7 +7817,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="270" spans="1:13">
+    <row r="270" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>1</v>
       </c>
@@ -7791,7 +7840,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="271" spans="1:13">
+    <row r="271" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>1</v>
       </c>
@@ -7817,7 +7866,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="272" spans="1:13">
+    <row r="272" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>17</v>
       </c>
@@ -7834,7 +7883,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="273" spans="1:13">
+    <row r="273" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>1</v>
       </c>
@@ -7857,7 +7906,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="274" spans="1:13">
+    <row r="274" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>3</v>
       </c>
@@ -7874,7 +7923,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="275" spans="1:13">
+    <row r="275" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>1</v>
       </c>
@@ -7897,7 +7946,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="276" spans="1:13">
+    <row r="276" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>1</v>
       </c>
@@ -7923,7 +7972,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="277" spans="1:13">
+    <row r="277" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>14</v>
       </c>
@@ -7937,7 +7986,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="278" spans="1:13">
+    <row r="278" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>1</v>
       </c>
@@ -7960,7 +8009,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="279" spans="1:13">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>3</v>
       </c>
@@ -7977,7 +8026,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="280" spans="1:13">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>1</v>
       </c>
@@ -8000,7 +8049,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="281" spans="1:13">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>1</v>
       </c>
@@ -8023,7 +8072,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="282" spans="1:13">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>14</v>
       </c>
@@ -8037,7 +8086,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="283" spans="1:13">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>1</v>
       </c>
@@ -8060,7 +8109,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="284" spans="1:13">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>7</v>
       </c>
@@ -8080,7 +8129,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="285" spans="1:13">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>1</v>
       </c>
@@ -8106,7 +8155,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="286" spans="1:13">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>14</v>
       </c>
@@ -8120,7 +8169,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="287" spans="1:13">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>14</v>
       </c>
@@ -8134,7 +8183,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="288" spans="1:13">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>1</v>
       </c>
@@ -8160,7 +8209,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="289" spans="1:13">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>1</v>
       </c>
@@ -8183,7 +8232,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="290" spans="1:13">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>14</v>
       </c>
@@ -8197,7 +8246,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="291" spans="1:13">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>1</v>
       </c>
@@ -8223,7 +8272,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="292" spans="1:13">
+    <row r="292" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>14</v>
       </c>
@@ -8237,7 +8286,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="293" spans="1:13">
+    <row r="293" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A293">
         <v>1</v>
       </c>
@@ -8263,7 +8312,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="294" spans="1:13">
+    <row r="294" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>17</v>
       </c>
@@ -8280,7 +8329,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="295" spans="1:13">
+    <row r="295" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>1</v>
       </c>
@@ -8303,7 +8352,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="296" spans="1:13">
+    <row r="296" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>1</v>
       </c>
@@ -8329,7 +8378,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="297" spans="1:13">
+    <row r="297" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>14</v>
       </c>
@@ -8343,7 +8392,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="298" spans="1:13">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>1</v>
       </c>
@@ -8366,7 +8415,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="299" spans="1:13">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>3</v>
       </c>
@@ -8383,7 +8432,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="300" spans="1:13">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>1</v>
       </c>
@@ -8406,7 +8455,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="301" spans="1:13">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>1</v>
       </c>
@@ -8432,7 +8481,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="302" spans="1:13">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>14</v>
       </c>
@@ -8446,7 +8495,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="303" spans="1:13">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>1</v>
       </c>
@@ -8469,7 +8518,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="304" spans="1:13">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>3</v>
       </c>
@@ -8486,7 +8535,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="305" spans="1:13">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>28</v>
       </c>
@@ -8503,7 +8552,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="306" spans="1:13">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>14</v>
       </c>
@@ -8517,7 +8566,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="307" spans="1:13">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>1</v>
       </c>
@@ -8540,7 +8589,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="308" spans="1:13">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>1</v>
       </c>
@@ -8566,7 +8615,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="309" spans="1:13">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>17</v>
       </c>
@@ -8583,7 +8632,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="310" spans="1:13">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>1</v>
       </c>
@@ -8609,7 +8658,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="311" spans="1:13">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>14</v>
       </c>
@@ -8623,7 +8672,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="312" spans="1:13">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A312">
         <v>3</v>
       </c>
@@ -8640,7 +8689,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="313" spans="1:13">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A313">
         <v>1</v>
       </c>
@@ -8663,7 +8712,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="314" spans="1:13">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A314">
         <v>14</v>
       </c>
@@ -8677,7 +8726,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="315" spans="1:13">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A315">
         <v>1</v>
       </c>
@@ -8703,7 +8752,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="316" spans="1:13">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A316">
         <v>1</v>
       </c>
@@ -8726,7 +8775,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="317" spans="1:13">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A317">
         <v>14</v>
       </c>
@@ -8740,7 +8789,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="318" spans="1:13">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A318">
         <v>1</v>
       </c>
@@ -8766,7 +8815,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="319" spans="1:13">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A319">
         <v>14</v>
       </c>
@@ -8780,7 +8829,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="320" spans="1:13">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A320">
         <v>1</v>
       </c>
@@ -8803,7 +8852,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="321" spans="1:13">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A321">
         <v>17</v>
       </c>
@@ -8823,7 +8872,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="322" spans="1:13">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A322">
         <v>1</v>
       </c>
@@ -8846,7 +8895,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="323" spans="1:13">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A323">
         <v>14</v>
       </c>
@@ -8860,7 +8909,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="324" spans="1:13">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A324">
         <v>1</v>
       </c>
@@ -8895,7 +8944,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="325" spans="1:13">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A325">
         <v>14</v>
       </c>
@@ -8909,7 +8958,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="326" spans="1:13">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A326">
         <v>1</v>
       </c>
@@ -8944,7 +8993,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="327" spans="1:13">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A327">
         <v>14</v>
       </c>
@@ -8958,7 +9007,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="328" spans="1:13">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A328">
         <v>1</v>
       </c>
@@ -8990,7 +9039,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="329" spans="1:13">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A329">
         <v>1</v>
       </c>
@@ -9025,7 +9074,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="330" spans="1:13">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A330">
         <v>14</v>
       </c>
@@ -9039,7 +9088,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="331" spans="1:13">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A331">
         <v>1</v>
       </c>
@@ -9071,7 +9120,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="332" spans="1:13">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A332">
         <v>17</v>
       </c>
@@ -9091,7 +9140,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="333" spans="1:13">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A333">
         <v>1</v>
       </c>
@@ -9123,7 +9172,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="334" spans="1:13">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A334">
         <v>1</v>
       </c>
@@ -9155,7 +9204,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="335" spans="1:13">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A335">
         <v>14</v>
       </c>
@@ -9169,7 +9218,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="336" spans="1:13">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A336">
         <v>3</v>
       </c>
@@ -9186,7 +9235,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="337" spans="1:13">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A337">
         <v>1</v>
       </c>
@@ -9218,7 +9267,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="338" spans="1:13">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A338">
         <v>14</v>
       </c>
@@ -9232,7 +9281,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="339" spans="1:13">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A339">
         <v>3</v>
       </c>
@@ -9249,7 +9298,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="340" spans="1:13">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A340">
         <v>14</v>
       </c>
@@ -9263,7 +9312,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="341" spans="1:13">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A341">
         <v>1</v>
       </c>
@@ -9298,7 +9347,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="342" spans="1:13">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A342">
         <v>14</v>
       </c>

</xml_diff>